<commit_message>
Change colors and add new logo. Almost done
</commit_message>
<xml_diff>
--- a/table2_2.xlsx
+++ b/table2_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto/Desktop/THESIS/HRS/git/icmla_poster/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reisanar/Google Drive/FL_Poly/research_and_other_publications/icmla_poster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19E7E6-7481-5042-A1A7-359DE0B2AF45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4276ABCE-FC0F-9F47-8895-105219FEB653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="960" windowWidth="24320" windowHeight="14500" xr2:uid="{50E23362-45C6-B34A-916D-137ECC0A9151}"/>
   </bookViews>
@@ -204,16 +204,16 @@
     <t>responsible A little</t>
   </si>
   <si>
-    <t>Dim 1</t>
-  </si>
-  <si>
-    <t>Dim 2</t>
-  </si>
-  <si>
-    <t>Dim 3</t>
-  </si>
-  <si>
-    <t>Dim 4</t>
+    <t>Dimension 1</t>
+  </si>
+  <si>
+    <t>Dimension 2</t>
+  </si>
+  <si>
+    <t>Dimension 3</t>
+  </si>
+  <si>
+    <t>Dimension 4</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>